<commit_message>
Update some info files
</commit_message>
<xml_diff>
--- a/Hardware/Parts Lists.xlsx
+++ b/Hardware/Parts Lists.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\EAGLE\projects\Divergence Meter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\KiCad\6.0\projects\Divergence Meter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12975" windowHeight="4845" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12975" windowHeight="4845" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tom Titor Parts List" sheetId="1" r:id="rId1"/>
     <sheet name="Component Update Parts List" sheetId="3" r:id="rId2"/>
-    <sheet name="Thru Design Update Parts List" sheetId="4" r:id="rId3"/>
-    <sheet name="Full SMT Redesign" sheetId="5" r:id="rId4"/>
+    <sheet name="Thru Hole Update Parts List" sheetId="4" r:id="rId3"/>
+    <sheet name="SMT Redesign" sheetId="5" r:id="rId4"/>
     <sheet name="Physical Construction" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="331">
   <si>
     <t>Quantity</t>
   </si>
@@ -750,9 +750,6 @@
     <t>Prices as of 6/12/21</t>
   </si>
   <si>
-    <t>667-EEU-FC1C331 per HVPS datasheet</t>
-  </si>
-  <si>
     <t>726-BAS7005WH6327</t>
   </si>
   <si>
@@ -780,9 +777,6 @@
     <t>7 Pin .1" Pitch Header Male</t>
   </si>
   <si>
-    <t>5 Pin .1" Pitch Header Female</t>
-  </si>
-  <si>
     <t>R4, R5</t>
   </si>
   <si>
@@ -840,9 +834,6 @@
     <t>Direct from Microchip is also an option</t>
   </si>
   <si>
-    <t xml:space="preserve">428-202677-MG01 </t>
-  </si>
-  <si>
     <t>Micro Crystal RV-8803-C7</t>
   </si>
   <si>
@@ -906,9 +897,6 @@
     <t>595-TLV76750QWDRBRQ1</t>
   </si>
   <si>
-    <t>TLV766-Q1 Fixed 5V Linear Voltage Regulator</t>
-  </si>
-  <si>
     <t>Power Adapter 9-12V</t>
   </si>
   <si>
@@ -1000,6 +988,39 @@
   </si>
   <si>
     <t>Debug only</t>
+  </si>
+  <si>
+    <t>TLV767-Q1 Fixed 5V Linear Voltage Regulator</t>
+  </si>
+  <si>
+    <t>U5, U6, U7</t>
+  </si>
+  <si>
+    <t>John at Taylor Electronics has oked this as a replacement for 667-EEU-FC1C331 per HVPS datasheet</t>
+  </si>
+  <si>
+    <t>428-202677-MG01</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://octopart.com/3519-keystone-45750?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/800-10-064-10-001000-mill-max-258892?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/801-41-050-10-001000-mill-max-25804236?r=sp</t>
+  </si>
+  <si>
+    <t>5 Pin .1" Pitch Header Male</t>
+  </si>
+  <si>
+    <t>NC1-4</t>
+  </si>
+  <si>
+    <t>NC5-8</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1386,6 +1407,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1400,9 +1431,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1686,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2101,10 +2129,10 @@
       <c r="C23" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="59" t="s">
+      <c r="D23" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="64" t="s">
         <v>38</v>
       </c>
       <c r="F23" s="17"/>
@@ -2119,8 +2147,8 @@
       <c r="C24" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="59"/>
-      <c r="E24" s="60"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="64"/>
       <c r="F24" s="17"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2133,8 +2161,8 @@
       <c r="C25" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="60"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
       <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2147,10 +2175,10 @@
       <c r="C26" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="59" t="s">
+      <c r="D26" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="60" t="s">
+      <c r="E26" s="64" t="s">
         <v>40</v>
       </c>
       <c r="F26" s="17"/>
@@ -2165,8 +2193,8 @@
       <c r="C27" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="60"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="64"/>
       <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,7 +2509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
@@ -2531,7 +2559,7 @@
       <c r="E2" s="32"/>
       <c r="F2" s="17"/>
       <c r="G2" s="21" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2581,7 +2609,7 @@
         <v>174</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G5" s="22"/>
     </row>
@@ -2602,7 +2630,7 @@
         <v>70</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G6" s="22"/>
     </row>
@@ -2623,7 +2651,7 @@
         <v>214</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="G7" s="22"/>
     </row>
@@ -2788,7 +2816,7 @@
         <v>184</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2808,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2864,7 +2892,7 @@
         <v>188</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -2884,7 +2912,7 @@
         <v>188</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2915,10 +2943,10 @@
       <c r="C23" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="59" t="s">
+      <c r="D23" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="64" t="s">
         <v>40</v>
       </c>
       <c r="F23" s="17"/>
@@ -2933,8 +2961,8 @@
       <c r="C24" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="59"/>
-      <c r="E24" s="60"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="64"/>
       <c r="F24" s="17"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2947,8 +2975,8 @@
       <c r="C25" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="60"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
       <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2961,10 +2989,10 @@
       <c r="C26" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="59" t="s">
+      <c r="D26" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="60" t="s">
+      <c r="E26" s="64" t="s">
         <v>190</v>
       </c>
       <c r="F26" s="17"/>
@@ -2979,8 +3007,8 @@
       <c r="C27" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="60"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="64"/>
       <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3000,7 +3028,7 @@
         <v>192</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3038,7 +3066,7 @@
         <v>194</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3058,7 +3086,7 @@
         <v>49</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3078,7 +3106,7 @@
         <v>198</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -3098,7 +3126,7 @@
         <v>200</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3118,7 +3146,7 @@
         <v>201</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -3138,7 +3166,7 @@
         <v>31</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -3156,7 +3184,7 @@
         <v>203</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -3196,7 +3224,7 @@
         <v>207</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3216,7 +3244,7 @@
         <v>212</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -3307,8 +3335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3683,10 +3711,10 @@
       <c r="C21" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="61" t="s">
+      <c r="D21" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="60" t="s">
+      <c r="E21" s="64" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="17"/>
@@ -3701,8 +3729,8 @@
       <c r="C22" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="60"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="64"/>
       <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3715,8 +3743,8 @@
       <c r="C23" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="60"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="64"/>
       <c r="F23" s="17"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3729,10 +3757,10 @@
       <c r="C24" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="D24" s="61" t="s">
+      <c r="D24" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="64" t="s">
         <v>190</v>
       </c>
       <c r="F24" s="17"/>
@@ -3747,8 +3775,8 @@
       <c r="C25" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="60"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="64"/>
       <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3851,7 +3879,7 @@
       <c r="C31" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="14" t="s">
         <v>223</v>
       </c>
       <c r="E31" s="11" t="s">
@@ -3876,7 +3904,7 @@
         <v>201</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -3896,7 +3924,7 @@
         <v>31</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4031,10 +4059,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4059,13 +4087,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>233</v>
+        <v>324</v>
       </c>
       <c r="E1" s="50" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>109</v>
@@ -4098,7 +4126,7 @@
         <v>232</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C3" s="47" t="s">
         <v>236</v>
@@ -4119,7 +4147,7 @@
         <v>138</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C4" s="47"/>
       <c r="D4" s="48"/>
@@ -4132,7 +4160,7 @@
         <v>228</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>236</v>
@@ -4147,21 +4175,21 @@
         <v>0.27</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C6" s="47" t="s">
         <v>236</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E6" s="18">
         <v>1</v>
@@ -4170,21 +4198,21 @@
         <v>0.26</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C7" s="47" t="s">
         <v>236</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E7" s="18">
         <v>3</v>
@@ -4193,7 +4221,7 @@
         <v>0.3</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4201,13 +4229,13 @@
         <v>97</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C8" s="57" t="s">
         <v>236</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E8" s="18">
         <v>1</v>
@@ -4222,13 +4250,13 @@
         <v>96</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C9" s="47" t="s">
         <v>236</v>
       </c>
       <c r="D9" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E9" s="18">
         <v>1</v>
@@ -4240,7 +4268,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B10" s="47" t="s">
         <v>238</v>
@@ -4258,15 +4286,15 @@
         <v>0.74</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>240</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C11" s="47" t="s">
         <v>236</v>
@@ -4287,7 +4315,7 @@
         <v>91</v>
       </c>
       <c r="B12" s="47" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C12" s="47" t="s">
         <v>236</v>
@@ -4309,13 +4337,13 @@
         <v>140</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C13" s="47" t="s">
         <v>236</v>
       </c>
       <c r="D13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E13" s="18">
         <v>1</v>
@@ -4324,7 +4352,7 @@
         <v>0.51</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="H13" s="22"/>
     </row>
@@ -4348,7 +4376,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4361,23 +4389,23 @@
       <c r="C15" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="D15" s="42" t="s">
-        <v>213</v>
+      <c r="D15" t="s">
+        <v>9</v>
       </c>
       <c r="E15" s="18">
         <v>1</v>
       </c>
       <c r="F15" s="54">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="G15" s="53" t="s">
+        <v>242</v>
+      </c>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
         <v>243</v>
-      </c>
-      <c r="H15" s="22"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
-        <v>244</v>
       </c>
       <c r="B16" s="47" t="s">
         <v>11</v>
@@ -4385,8 +4413,8 @@
       <c r="C16" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="D16" s="48" t="s">
-        <v>12</v>
+      <c r="D16" s="60" t="s">
+        <v>325</v>
       </c>
       <c r="E16" s="18">
         <v>2</v>
@@ -4395,20 +4423,19 @@
         <v>0.25</v>
       </c>
       <c r="G16" s="53"/>
-      <c r="H16" s="22"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
         <v>99</v>
       </c>
       <c r="B17" s="47" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="D17" s="48" t="s">
-        <v>37</v>
+      <c r="D17" s="60" t="s">
+        <v>327</v>
       </c>
       <c r="E17" s="18">
         <v>1</v>
@@ -4417,21 +4444,21 @@
         <v>8.39</v>
       </c>
       <c r="G17" s="53" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
         <v>92</v>
       </c>
       <c r="B18" s="47" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C18" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="D18" s="48" t="s">
-        <v>39</v>
+      <c r="D18" s="60" t="s">
+        <v>326</v>
       </c>
       <c r="E18" s="18">
         <v>1</v>
@@ -4440,15 +4467,15 @@
         <v>7.24</v>
       </c>
       <c r="G18" s="53" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
         <v>124</v>
       </c>
       <c r="B19" s="47" t="s">
-        <v>250</v>
+        <v>328</v>
       </c>
       <c r="C19" s="47" t="s">
         <v>236</v>
@@ -4462,7 +4489,7 @@
       <c r="F19" s="18"/>
       <c r="G19" s="53"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="47" t="s">
         <v>150</v>
       </c>
@@ -4485,18 +4512,18 @@
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
-        <v>125</v>
+        <v>329</v>
       </c>
       <c r="B21" s="47" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C21" s="47" t="s">
         <v>236</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E21" s="18">
         <v>3</v>
@@ -4504,28 +4531,29 @@
       <c r="F21" s="18"/>
       <c r="G21" s="53"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="47" t="s">
-        <v>149</v>
+        <v>330</v>
       </c>
       <c r="B22" s="47" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C22" s="47" t="s">
         <v>236</v>
       </c>
       <c r="D22" s="48" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E22" s="18">
         <v>3</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="53"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="61"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B23" s="47" t="s">
         <v>119</v>
@@ -4534,7 +4562,7 @@
         <v>236</v>
       </c>
       <c r="D23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E23" s="18">
         <v>5</v>
@@ -4543,21 +4571,21 @@
         <v>0.11</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="47" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B24" s="47" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C24" s="47" t="s">
         <v>236</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E24" s="18">
         <v>2</v>
@@ -4567,7 +4595,7 @@
       </c>
       <c r="G24" s="53"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
         <v>141</v>
       </c>
@@ -4578,7 +4606,7 @@
         <v>236</v>
       </c>
       <c r="D25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E25" s="18">
         <v>1</v>
@@ -4588,9 +4616,9 @@
       </c>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="47" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B26" s="47" t="s">
         <v>123</v>
@@ -4609,9 +4637,9 @@
       </c>
       <c r="G26" s="17"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="47" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B27" s="47" t="s">
         <v>143</v>
@@ -4629,12 +4657,13 @@
         <v>0.15</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="K27" s="61"/>
+    </row>
+    <row r="28" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="47" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B28" s="47" t="s">
         <v>122</v>
@@ -4643,7 +4672,7 @@
         <v>236</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E28" s="18">
         <v>16</v>
@@ -4652,12 +4681,12 @@
         <v>0.255</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="47" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B29" s="47" t="s">
         <v>121</v>
@@ -4666,7 +4695,7 @@
         <v>236</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E29" s="18">
         <v>8</v>
@@ -4676,7 +4705,7 @@
       </c>
       <c r="G29" s="17"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="47" t="s">
         <v>134</v>
       </c>
@@ -4692,12 +4721,12 @@
       <c r="E30" s="18">
         <v>2</v>
       </c>
-      <c r="F30" s="54">
-        <v>0.28000000000000003</v>
+      <c r="F30" s="62" t="s">
+        <v>236</v>
       </c>
       <c r="G30" s="17"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="47" t="s">
         <v>137</v>
       </c>
@@ -4718,7 +4747,7 @@
       </c>
       <c r="G31" s="17"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="47" t="s">
         <v>113</v>
       </c>
@@ -4729,7 +4758,7 @@
         <v>84</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E32" s="18">
         <v>8</v>
@@ -4742,18 +4771,18 @@
         <v>113</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>295</v>
-      </c>
-      <c r="C33" s="62" t="s">
-        <v>296</v>
-      </c>
-      <c r="D33" s="63"/>
+        <v>291</v>
+      </c>
+      <c r="C33" s="66" t="s">
+        <v>292</v>
+      </c>
+      <c r="D33" s="67"/>
       <c r="E33" s="18">
         <v>104</v>
       </c>
       <c r="F33" s="18"/>
       <c r="G33" s="18" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4761,13 +4790,13 @@
         <v>88</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>292</v>
+        <v>320</v>
       </c>
       <c r="C34" s="47" t="s">
         <v>236</v>
       </c>
       <c r="D34" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E34" s="18">
         <v>1</v>
@@ -4804,7 +4833,7 @@
         <v>87</v>
       </c>
       <c r="B36" s="47" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C36" s="47" t="s">
         <v>236</v>
@@ -4819,21 +4848,21 @@
         <v>1.27</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C37" s="47" t="s">
         <v>236</v>
       </c>
       <c r="D37" t="s">
-        <v>270</v>
+        <v>323</v>
       </c>
       <c r="E37" s="17">
         <v>1</v>
@@ -4842,21 +4871,21 @@
         <v>2.96</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="47" t="s">
-        <v>155</v>
+        <v>321</v>
       </c>
       <c r="B38" s="47" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C38" s="47" t="s">
         <v>236</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E38" s="18">
         <v>3</v>
@@ -4895,13 +4924,13 @@
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="47"/>
       <c r="B41" s="47" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C41" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="D41" s="64" t="s">
-        <v>300</v>
+      <c r="D41" s="59" t="s">
+        <v>296</v>
       </c>
       <c r="E41" s="18">
         <v>1</v>
@@ -4910,7 +4939,7 @@
         <v>12.5</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -5106,7 +5135,7 @@
         <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -5114,13 +5143,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D11" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>